<commit_message>
Perubahan nama variabel di jps optimize
</commit_message>
<xml_diff>
--- a/Excel/TanpaELL/HASIL-Rata-Semua-Map.xlsx
+++ b/Excel/TanpaELL/HASIL-Rata-Semua-Map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEMHAS\TA_Python_Server\Excel\TanpaELL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{082CD923-498D-4A62-8461-740A5A9A3765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619E4DBE-B9DE-41FA-858C-01F0BFB23FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{47726F7C-0459-43C3-A3D2-EC30F73D973E}"/>
   </bookViews>
@@ -272,7 +272,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,6 +282,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -335,10 +341,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -658,7 +667,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -716,7 +725,7 @@
         <v>2.9666750000000002E-3</v>
       </c>
       <c r="H2">
-        <f>AVERAGE(C2:G2)</f>
+        <f t="shared" ref="H2:H33" si="0">AVERAGE(C2:G2)</f>
         <v>3.2397449999999996E-3</v>
       </c>
     </row>
@@ -743,7 +752,7 @@
         <v>3.2720499999999999E-3</v>
       </c>
       <c r="H3">
-        <f>AVERAGE(C3:G3)</f>
+        <f t="shared" si="0"/>
         <v>3.3643950000000001E-3</v>
       </c>
     </row>
@@ -770,7 +779,7 @@
         <v>3.316275E-3</v>
       </c>
       <c r="H4">
-        <f>AVERAGE(C4:G4)</f>
+        <f t="shared" si="0"/>
         <v>3.5875950000000003E-3</v>
       </c>
     </row>
@@ -797,7 +806,7 @@
         <v>2.969775E-3</v>
       </c>
       <c r="H5">
-        <f>AVERAGE(C5:G5)</f>
+        <f t="shared" si="0"/>
         <v>3.607205E-3</v>
       </c>
     </row>
@@ -824,7 +833,7 @@
         <v>4.8440000000000002E-3</v>
       </c>
       <c r="H6">
-        <f>AVERAGE(C6:G6)</f>
+        <f t="shared" si="0"/>
         <v>3.9157050000000002E-3</v>
       </c>
     </row>
@@ -851,7 +860,7 @@
         <v>4.8699750000000003E-3</v>
       </c>
       <c r="H7">
-        <f>AVERAGE(C7:G7)</f>
+        <f t="shared" si="0"/>
         <v>4.0283100000000002E-3</v>
       </c>
     </row>
@@ -878,7 +887,7 @@
         <v>5.2357500000000008E-3</v>
       </c>
       <c r="H8">
-        <f>AVERAGE(C8:G8)</f>
+        <f t="shared" si="0"/>
         <v>4.0888950000000004E-3</v>
       </c>
     </row>
@@ -905,7 +914,7 @@
         <v>4.9431249999999996E-3</v>
       </c>
       <c r="H9">
-        <f>AVERAGE(C9:G9)</f>
+        <f t="shared" si="0"/>
         <v>4.1848600000000003E-3</v>
       </c>
     </row>
@@ -932,7 +941,7 @@
         <v>5.3484250000000004E-3</v>
       </c>
       <c r="H10">
-        <f>AVERAGE(C10:G10)</f>
+        <f t="shared" si="0"/>
         <v>4.4926100000000002E-3</v>
       </c>
     </row>
@@ -959,7 +968,7 @@
         <v>5.5235249999999996E-3</v>
       </c>
       <c r="H11">
-        <f>AVERAGE(C11:G11)</f>
+        <f t="shared" si="0"/>
         <v>4.5474300000000007E-3</v>
       </c>
     </row>
@@ -986,7 +995,7 @@
         <v>5.4184000000000003E-3</v>
       </c>
       <c r="H12">
-        <f>AVERAGE(C12:G12)</f>
+        <f t="shared" si="0"/>
         <v>4.5913099999999995E-3</v>
       </c>
     </row>
@@ -1013,7 +1022,7 @@
         <v>5.3650750000000004E-3</v>
       </c>
       <c r="H13">
-        <f>AVERAGE(C13:G13)</f>
+        <f t="shared" si="0"/>
         <v>4.766925E-3</v>
       </c>
     </row>
@@ -1040,7 +1049,7 @@
         <v>6.8058499999999996E-3</v>
       </c>
       <c r="H14">
-        <f>AVERAGE(C14:G14)</f>
+        <f t="shared" si="0"/>
         <v>4.9390200000000006E-3</v>
       </c>
     </row>
@@ -1067,7 +1076,7 @@
         <v>5.8628499999999993E-3</v>
       </c>
       <c r="H15">
-        <f>AVERAGE(C15:G15)</f>
+        <f t="shared" si="0"/>
         <v>4.9674699999999999E-3</v>
       </c>
     </row>
@@ -1094,7 +1103,7 @@
         <v>6.8995750000000007E-3</v>
       </c>
       <c r="H16">
-        <f>AVERAGE(C16:G16)</f>
+        <f t="shared" si="0"/>
         <v>5.1091799999999996E-3</v>
       </c>
     </row>
@@ -1102,7 +1111,7 @@
       <c r="A17" s="3">
         <v>4</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C17">
@@ -1121,7 +1130,7 @@
         <v>6.917824999999999E-3</v>
       </c>
       <c r="H17">
-        <f>AVERAGE(C17:G17)</f>
+        <f t="shared" si="0"/>
         <v>5.1190450000000009E-3</v>
       </c>
     </row>
@@ -1129,7 +1138,7 @@
       <c r="A18" s="3">
         <v>5</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C18">
@@ -1148,7 +1157,7 @@
         <v>7.0571999999999996E-3</v>
       </c>
       <c r="H18">
-        <f>AVERAGE(C18:G18)</f>
+        <f t="shared" si="0"/>
         <v>5.2225550000000003E-3</v>
       </c>
     </row>
@@ -1175,7 +1184,7 @@
         <v>6.9231999999999991E-3</v>
       </c>
       <c r="H19">
-        <f>AVERAGE(C19:G19)</f>
+        <f t="shared" si="0"/>
         <v>5.2512799999999997E-3</v>
       </c>
     </row>
@@ -1202,7 +1211,7 @@
         <v>6.84215E-3</v>
       </c>
       <c r="H20">
-        <f>AVERAGE(C20:G20)</f>
+        <f t="shared" si="0"/>
         <v>5.4146700000000008E-3</v>
       </c>
     </row>
@@ -1229,7 +1238,7 @@
         <v>5.489875E-3</v>
       </c>
       <c r="H21">
-        <f>AVERAGE(C21:G21)</f>
+        <f t="shared" si="0"/>
         <v>5.4724850000000009E-3</v>
       </c>
     </row>
@@ -1256,7 +1265,7 @@
         <v>7.5089750000000002E-3</v>
       </c>
       <c r="H22">
-        <f>AVERAGE(C22:G22)</f>
+        <f t="shared" si="0"/>
         <v>5.6456650000000011E-3</v>
       </c>
     </row>
@@ -1283,7 +1292,7 @@
         <v>7.9867749999999998E-3</v>
       </c>
       <c r="H23">
-        <f>AVERAGE(C23:G23)</f>
+        <f t="shared" si="0"/>
         <v>5.6541000000000004E-3</v>
       </c>
     </row>
@@ -1310,7 +1319,7 @@
         <v>7.5525999999999996E-3</v>
       </c>
       <c r="H24">
-        <f>AVERAGE(C24:G24)</f>
+        <f t="shared" si="0"/>
         <v>5.6572949999999997E-3</v>
       </c>
     </row>
@@ -1337,7 +1346,7 @@
         <v>5.6094250000000003E-3</v>
       </c>
       <c r="H25">
-        <f>AVERAGE(C25:G25)</f>
+        <f t="shared" si="0"/>
         <v>5.8869350000000003E-3</v>
       </c>
     </row>
@@ -1364,7 +1373,7 @@
         <v>7.5755750000000011E-3</v>
       </c>
       <c r="H26">
-        <f>AVERAGE(C26:G26)</f>
+        <f t="shared" si="0"/>
         <v>5.9525800000000007E-3</v>
       </c>
     </row>
@@ -1391,7 +1400,7 @@
         <v>7.7226999999999999E-3</v>
       </c>
       <c r="H27">
-        <f>AVERAGE(C27:G27)</f>
+        <f t="shared" si="0"/>
         <v>6.1470550000000002E-3</v>
       </c>
     </row>
@@ -1418,7 +1427,7 @@
         <v>5.1858E-3</v>
       </c>
       <c r="H28">
-        <f>AVERAGE(C28:G28)</f>
+        <f t="shared" si="0"/>
         <v>6.1972650000000004E-3</v>
       </c>
     </row>
@@ -1445,7 +1454,7 @@
         <v>8.5280499999999988E-3</v>
       </c>
       <c r="H29">
-        <f>AVERAGE(C29:G29)</f>
+        <f t="shared" si="0"/>
         <v>6.2638649999999987E-3</v>
       </c>
     </row>
@@ -1472,7 +1481,7 @@
         <v>8.8678250000000011E-3</v>
       </c>
       <c r="H30">
-        <f>AVERAGE(C30:G30)</f>
+        <f t="shared" si="0"/>
         <v>6.4633799999999995E-3</v>
       </c>
     </row>
@@ -1499,7 +1508,7 @@
         <v>8.8505000000000007E-3</v>
       </c>
       <c r="H31">
-        <f>AVERAGE(C31:G31)</f>
+        <f t="shared" si="0"/>
         <v>6.6772100000000003E-3</v>
       </c>
     </row>
@@ -1526,7 +1535,7 @@
         <v>7.2307250000000003E-3</v>
       </c>
       <c r="H32">
-        <f>AVERAGE(C32:G32)</f>
+        <f t="shared" si="0"/>
         <v>6.6922250000000013E-3</v>
       </c>
     </row>
@@ -1553,7 +1562,7 @@
         <v>7.81775E-3</v>
       </c>
       <c r="H33">
-        <f>AVERAGE(C33:G33)</f>
+        <f t="shared" si="0"/>
         <v>7.0144550000000002E-3</v>
       </c>
     </row>
@@ -1580,7 +1589,7 @@
         <v>7.3810749999999991E-3</v>
       </c>
       <c r="H34">
-        <f>AVERAGE(C34:G34)</f>
+        <f t="shared" ref="H34:H65" si="1">AVERAGE(C34:G34)</f>
         <v>7.4933299999999994E-3</v>
       </c>
     </row>
@@ -1607,7 +1616,7 @@
         <v>7.8410500000000005E-3</v>
       </c>
       <c r="H35">
-        <f>AVERAGE(C35:G35)</f>
+        <f t="shared" si="1"/>
         <v>7.527294999999999E-3</v>
       </c>
     </row>
@@ -1634,7 +1643,7 @@
         <v>7.5716250000000002E-3</v>
       </c>
       <c r="H36">
-        <f>AVERAGE(C36:G36)</f>
+        <f t="shared" si="1"/>
         <v>7.6169699999999989E-3</v>
       </c>
     </row>
@@ -1661,7 +1670,7 @@
         <v>7.7641250000000011E-3</v>
       </c>
       <c r="H37">
-        <f>AVERAGE(C37:G37)</f>
+        <f t="shared" si="1"/>
         <v>7.9287550000000009E-3</v>
       </c>
     </row>
@@ -1688,7 +1697,7 @@
         <v>8.4218500000000016E-3</v>
       </c>
       <c r="H38">
-        <f>AVERAGE(C38:G38)</f>
+        <f t="shared" si="1"/>
         <v>7.961010000000001E-3</v>
       </c>
     </row>
@@ -1715,7 +1724,7 @@
         <v>9.2545749999999993E-3</v>
       </c>
       <c r="H39">
-        <f>AVERAGE(C39:G39)</f>
+        <f t="shared" si="1"/>
         <v>8.0952200000000002E-3</v>
       </c>
     </row>
@@ -1742,7 +1751,7 @@
         <v>8.0068750000000001E-3</v>
       </c>
       <c r="H40">
-        <f>AVERAGE(C40:G40)</f>
+        <f t="shared" si="1"/>
         <v>8.1469400000000001E-3</v>
       </c>
     </row>
@@ -1769,7 +1778,7 @@
         <v>8.4601499999999996E-3</v>
       </c>
       <c r="H41">
-        <f>AVERAGE(C41:G41)</f>
+        <f t="shared" si="1"/>
         <v>8.2300399999999992E-3</v>
       </c>
     </row>
@@ -1796,7 +1805,7 @@
         <v>8.3695750000000006E-3</v>
       </c>
       <c r="H42">
-        <f>AVERAGE(C42:G42)</f>
+        <f t="shared" si="1"/>
         <v>1.1466490000000001E-2</v>
       </c>
     </row>
@@ -1823,7 +1832,7 @@
         <v>9.5082750000000001E-3</v>
       </c>
       <c r="H43">
-        <f>AVERAGE(C43:G43)</f>
+        <f t="shared" si="1"/>
         <v>1.1682395000000002E-2</v>
       </c>
     </row>
@@ -1850,7 +1859,7 @@
         <v>9.2666499999999995E-3</v>
       </c>
       <c r="H44">
-        <f>AVERAGE(C44:G44)</f>
+        <f t="shared" si="1"/>
         <v>1.188608E-2</v>
       </c>
     </row>
@@ -1877,7 +1886,7 @@
         <v>9.7596000000000002E-3</v>
       </c>
       <c r="H45">
-        <f>AVERAGE(C45:G45)</f>
+        <f t="shared" si="1"/>
         <v>1.2435555000000001E-2</v>
       </c>
     </row>
@@ -1904,7 +1913,7 @@
         <v>9.9568E-3</v>
       </c>
       <c r="H46">
-        <f>AVERAGE(C46:G46)</f>
+        <f t="shared" si="1"/>
         <v>1.4452185000000001E-2</v>
       </c>
     </row>
@@ -1931,7 +1940,7 @@
         <v>9.9590249999999998E-3</v>
       </c>
       <c r="H47">
-        <f>AVERAGE(C47:G47)</f>
+        <f t="shared" si="1"/>
         <v>1.449281E-2</v>
       </c>
     </row>
@@ -1958,7 +1967,7 @@
         <v>1.0398575E-2</v>
       </c>
       <c r="H48">
-        <f>AVERAGE(C48:G48)</f>
+        <f t="shared" si="1"/>
         <v>1.5407725000000001E-2</v>
       </c>
     </row>
@@ -1985,7 +1994,7 @@
         <v>1.210285E-2</v>
       </c>
       <c r="H49">
-        <f>AVERAGE(C49:G49)</f>
+        <f t="shared" si="1"/>
         <v>1.5866999999999999E-2</v>
       </c>
     </row>
@@ -2012,7 +2021,7 @@
         <v>1.0264225E-2</v>
       </c>
       <c r="H50">
-        <f>AVERAGE(C50:G50)</f>
+        <f t="shared" si="1"/>
         <v>2.3817120000000004E-2</v>
       </c>
     </row>
@@ -2039,7 +2048,7 @@
         <v>1.1613399999999999E-2</v>
       </c>
       <c r="H51">
-        <f>AVERAGE(C51:G51)</f>
+        <f t="shared" si="1"/>
         <v>2.4388319999999998E-2</v>
       </c>
     </row>
@@ -2066,7 +2075,7 @@
         <v>1.0697824999999999E-2</v>
       </c>
       <c r="H52">
-        <f>AVERAGE(C52:G52)</f>
+        <f t="shared" si="1"/>
         <v>2.4759029999999998E-2</v>
       </c>
     </row>
@@ -2093,7 +2102,7 @@
         <v>1.0717025E-2</v>
       </c>
       <c r="H53">
-        <f>AVERAGE(C53:G53)</f>
+        <f t="shared" si="1"/>
         <v>2.4989640000000004E-2</v>
       </c>
     </row>
@@ -2120,7 +2129,7 @@
         <v>2.0468199999999999E-2</v>
       </c>
       <c r="H54">
-        <f>AVERAGE(C54:G54)</f>
+        <f t="shared" si="1"/>
         <v>2.8815995E-2</v>
       </c>
     </row>
@@ -2147,7 +2156,7 @@
         <v>1.7102525E-2</v>
       </c>
       <c r="H55">
-        <f>AVERAGE(C55:G55)</f>
+        <f t="shared" si="1"/>
         <v>3.045519E-2</v>
       </c>
     </row>
@@ -2174,7 +2183,7 @@
         <v>1.7528999999999999E-2</v>
       </c>
       <c r="H56">
-        <f>AVERAGE(C56:G56)</f>
+        <f t="shared" si="1"/>
         <v>3.4104790000000003E-2</v>
       </c>
     </row>
@@ -2201,7 +2210,7 @@
         <v>2.1173475000000001E-2</v>
       </c>
       <c r="H57">
-        <f>AVERAGE(C57:G57)</f>
+        <f t="shared" si="1"/>
         <v>3.5784849999999993E-2</v>
       </c>
     </row>
@@ -2228,7 +2237,7 @@
         <v>4.5767875E-2</v>
       </c>
       <c r="H58">
-        <f>AVERAGE(C58:G58)</f>
+        <f t="shared" si="1"/>
         <v>3.8662185000000002E-2</v>
       </c>
     </row>
@@ -2255,7 +2264,7 @@
         <v>4.2758474999999997E-2</v>
       </c>
       <c r="H59">
-        <f>AVERAGE(C59:G59)</f>
+        <f t="shared" si="1"/>
         <v>4.0692655000000001E-2</v>
       </c>
     </row>
@@ -2282,7 +2291,7 @@
         <v>4.7016124999999999E-2</v>
       </c>
       <c r="H60">
-        <f>AVERAGE(C60:G60)</f>
+        <f t="shared" si="1"/>
         <v>4.3256414999999999E-2</v>
       </c>
     </row>
@@ -2309,7 +2318,7 @@
         <v>4.3308500000000007E-2</v>
       </c>
       <c r="H61">
-        <f>AVERAGE(C61:G61)</f>
+        <f t="shared" si="1"/>
         <v>4.5771559999999996E-2</v>
       </c>
     </row>
@@ -2336,7 +2345,7 @@
         <v>9.5510700000000004E-2</v>
       </c>
       <c r="H62">
-        <f>AVERAGE(C62:G62)</f>
+        <f t="shared" si="1"/>
         <v>5.4831040000000011E-2</v>
       </c>
     </row>
@@ -2363,7 +2372,7 @@
         <v>9.4515624999999992E-2</v>
       </c>
       <c r="H63">
-        <f>AVERAGE(C63:G63)</f>
+        <f t="shared" si="1"/>
         <v>5.5754139999999994E-2</v>
       </c>
     </row>
@@ -2390,7 +2399,7 @@
         <v>9.787182500000001E-2</v>
       </c>
       <c r="H64">
-        <f>AVERAGE(C64:G64)</f>
+        <f t="shared" si="1"/>
         <v>5.9060605000000002E-2</v>
       </c>
     </row>
@@ -2417,7 +2426,7 @@
         <v>9.7145474999999995E-2</v>
       </c>
       <c r="H65">
-        <f>AVERAGE(C65:G65)</f>
+        <f t="shared" si="1"/>
         <v>6.1555634999999997E-2</v>
       </c>
     </row>
@@ -2436,7 +2445,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2495,7 +2504,7 @@
         <v>2</v>
       </c>
       <c r="H2" s="3">
-        <f>AVERAGE(C2:G2)</f>
+        <f t="shared" ref="H2:H33" si="0">AVERAGE(C2:G2)</f>
         <v>6.75</v>
       </c>
     </row>
@@ -2522,7 +2531,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="3">
-        <f>AVERAGE(C3:G3)</f>
+        <f t="shared" si="0"/>
         <v>6.75</v>
       </c>
     </row>
@@ -2549,7 +2558,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="3">
-        <f>AVERAGE(C4:G4)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -2576,7 +2585,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="3">
-        <f>AVERAGE(C5:G5)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -2603,7 +2612,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="3">
-        <f>AVERAGE(C6:G6)</f>
+        <f t="shared" si="0"/>
         <v>7.15</v>
       </c>
     </row>
@@ -2630,7 +2639,7 @@
         <v>2</v>
       </c>
       <c r="H7" s="3">
-        <f>AVERAGE(C7:G7)</f>
+        <f t="shared" si="0"/>
         <v>7.2</v>
       </c>
     </row>
@@ -2657,7 +2666,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="3">
-        <f>AVERAGE(C8:G8)</f>
+        <f t="shared" si="0"/>
         <v>7.7</v>
       </c>
     </row>
@@ -2684,7 +2693,7 @@
         <v>2.5</v>
       </c>
       <c r="H9" s="3">
-        <f>AVERAGE(C9:G9)</f>
+        <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
     </row>
@@ -2692,7 +2701,7 @@
       <c r="A10" s="3">
         <v>4</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C10">
@@ -2711,7 +2720,7 @@
         <v>2.75</v>
       </c>
       <c r="H10" s="3">
-        <f>AVERAGE(C10:G10)</f>
+        <f t="shared" si="0"/>
         <v>7.8</v>
       </c>
     </row>
@@ -2738,7 +2747,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="3">
-        <f>AVERAGE(C11:G11)</f>
+        <f t="shared" si="0"/>
         <v>7.85</v>
       </c>
     </row>
@@ -2765,7 +2774,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="3">
-        <f>AVERAGE(C12:G12)</f>
+        <f t="shared" si="0"/>
         <v>7.9</v>
       </c>
     </row>
@@ -2792,7 +2801,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="3">
-        <f>AVERAGE(C13:G13)</f>
+        <f t="shared" si="0"/>
         <v>7.95</v>
       </c>
     </row>
@@ -2819,7 +2828,7 @@
         <v>4</v>
       </c>
       <c r="H14" s="3">
-        <f>AVERAGE(C14:G14)</f>
+        <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
     </row>
@@ -2846,7 +2855,7 @@
         <v>2.75</v>
       </c>
       <c r="H15" s="3">
-        <f>AVERAGE(C15:G15)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
     </row>
@@ -2873,7 +2882,7 @@
         <v>3.25</v>
       </c>
       <c r="H16" s="3">
-        <f>AVERAGE(C16:G16)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
     </row>
@@ -2900,7 +2909,7 @@
         <v>4</v>
       </c>
       <c r="H17" s="3">
-        <f>AVERAGE(C17:G17)</f>
+        <f t="shared" si="0"/>
         <v>8.5500000000000007</v>
       </c>
     </row>
@@ -2927,7 +2936,7 @@
         <v>4</v>
       </c>
       <c r="H18" s="3">
-        <f>AVERAGE(C18:G18)</f>
+        <f t="shared" si="0"/>
         <v>8.6</v>
       </c>
     </row>
@@ -2954,7 +2963,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="3">
-        <f>AVERAGE(C19:G19)</f>
+        <f t="shared" si="0"/>
         <v>8.8000000000000007</v>
       </c>
     </row>
@@ -2981,7 +2990,7 @@
         <v>2.5</v>
       </c>
       <c r="H20" s="3">
-        <f>AVERAGE(C20:G20)</f>
+        <f t="shared" si="0"/>
         <v>8.9</v>
       </c>
     </row>
@@ -3008,7 +3017,7 @@
         <v>4.75</v>
       </c>
       <c r="H21" s="3">
-        <f>AVERAGE(C21:G21)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -3035,7 +3044,7 @@
         <v>4.75</v>
       </c>
       <c r="H22" s="3">
-        <f>AVERAGE(C22:G22)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -3062,7 +3071,7 @@
         <v>3.75</v>
       </c>
       <c r="H23" s="3">
-        <f>AVERAGE(C23:G23)</f>
+        <f t="shared" si="0"/>
         <v>9.0500000000000007</v>
       </c>
     </row>
@@ -3089,7 +3098,7 @@
         <v>4.75</v>
       </c>
       <c r="H24" s="3">
-        <f>AVERAGE(C24:G24)</f>
+        <f t="shared" si="0"/>
         <v>9.1</v>
       </c>
     </row>
@@ -3116,7 +3125,7 @@
         <v>4.25</v>
       </c>
       <c r="H25" s="3">
-        <f>AVERAGE(C25:G25)</f>
+        <f t="shared" si="0"/>
         <v>9.1</v>
       </c>
     </row>
@@ -3143,7 +3152,7 @@
         <v>4.75</v>
       </c>
       <c r="H26" s="3">
-        <f>AVERAGE(C26:G26)</f>
+        <f t="shared" si="0"/>
         <v>9.1</v>
       </c>
     </row>
@@ -3170,7 +3179,7 @@
         <v>5.25</v>
       </c>
       <c r="H27" s="3">
-        <f>AVERAGE(C27:G27)</f>
+        <f t="shared" si="0"/>
         <v>9.15</v>
       </c>
     </row>
@@ -3197,7 +3206,7 @@
         <v>4.75</v>
       </c>
       <c r="H28" s="3">
-        <f>AVERAGE(C28:G28)</f>
+        <f t="shared" si="0"/>
         <v>9.15</v>
       </c>
     </row>
@@ -3224,7 +3233,7 @@
         <v>2.75</v>
       </c>
       <c r="H29" s="3">
-        <f>AVERAGE(C29:G29)</f>
+        <f t="shared" si="0"/>
         <v>9.1999999999999993</v>
       </c>
     </row>
@@ -3251,7 +3260,7 @@
         <v>5</v>
       </c>
       <c r="H30" s="3">
-        <f>AVERAGE(C30:G30)</f>
+        <f t="shared" si="0"/>
         <v>9.25</v>
       </c>
     </row>
@@ -3278,7 +3287,7 @@
         <v>5</v>
       </c>
       <c r="H31" s="3">
-        <f>AVERAGE(C31:G31)</f>
+        <f t="shared" si="0"/>
         <v>9.3000000000000007</v>
       </c>
     </row>
@@ -3305,7 +3314,7 @@
         <v>4.75</v>
       </c>
       <c r="H32" s="3">
-        <f>AVERAGE(C32:G32)</f>
+        <f t="shared" si="0"/>
         <v>9.3000000000000007</v>
       </c>
     </row>
@@ -3332,7 +3341,7 @@
         <v>5.25</v>
       </c>
       <c r="H33" s="3">
-        <f>AVERAGE(C33:G33)</f>
+        <f t="shared" si="0"/>
         <v>9.35</v>
       </c>
     </row>
@@ -3359,7 +3368,7 @@
         <v>6.25</v>
       </c>
       <c r="H34" s="3">
-        <f>AVERAGE(C34:G34)</f>
+        <f t="shared" ref="H34:H65" si="1">AVERAGE(C34:G34)</f>
         <v>9.35</v>
       </c>
     </row>
@@ -3386,7 +3395,7 @@
         <v>4.75</v>
       </c>
       <c r="H35" s="3">
-        <f>AVERAGE(C35:G35)</f>
+        <f t="shared" si="1"/>
         <v>9.4</v>
       </c>
     </row>
@@ -3413,7 +3422,7 @@
         <v>4.75</v>
       </c>
       <c r="H36" s="3">
-        <f>AVERAGE(C36:G36)</f>
+        <f t="shared" si="1"/>
         <v>9.4</v>
       </c>
     </row>
@@ -3440,7 +3449,7 @@
         <v>2.75</v>
       </c>
       <c r="H37" s="3">
-        <f>AVERAGE(C37:G37)</f>
+        <f t="shared" si="1"/>
         <v>9.6</v>
       </c>
     </row>
@@ -3467,7 +3476,7 @@
         <v>4.25</v>
       </c>
       <c r="H38" s="3">
-        <f>AVERAGE(C38:G38)</f>
+        <f t="shared" si="1"/>
         <v>9.6</v>
       </c>
     </row>
@@ -3494,7 +3503,7 @@
         <v>4.5</v>
       </c>
       <c r="H39" s="3">
-        <f>AVERAGE(C39:G39)</f>
+        <f t="shared" si="1"/>
         <v>9.65</v>
       </c>
     </row>
@@ -3521,7 +3530,7 @@
         <v>4.5</v>
       </c>
       <c r="H40" s="3">
-        <f>AVERAGE(C40:G40)</f>
+        <f t="shared" si="1"/>
         <v>10.25</v>
       </c>
     </row>
@@ -3548,7 +3557,7 @@
         <v>6.75</v>
       </c>
       <c r="H41" s="3">
-        <f>AVERAGE(C41:G41)</f>
+        <f t="shared" si="1"/>
         <v>10.85</v>
       </c>
     </row>
@@ -3575,7 +3584,7 @@
         <v>6.75</v>
       </c>
       <c r="H42" s="3">
-        <f>AVERAGE(C42:G42)</f>
+        <f t="shared" si="1"/>
         <v>10.85</v>
       </c>
     </row>
@@ -3602,7 +3611,7 @@
         <v>4.25</v>
       </c>
       <c r="H43" s="3">
-        <f>AVERAGE(C43:G43)</f>
+        <f t="shared" si="1"/>
         <v>10.9</v>
       </c>
     </row>
@@ -3629,7 +3638,7 @@
         <v>6.75</v>
       </c>
       <c r="H44" s="3">
-        <f>AVERAGE(C44:G44)</f>
+        <f t="shared" si="1"/>
         <v>11.2</v>
       </c>
     </row>
@@ -3656,7 +3665,7 @@
         <v>6.75</v>
       </c>
       <c r="H45" s="3">
-        <f>AVERAGE(C45:G45)</f>
+        <f t="shared" si="1"/>
         <v>11.2</v>
       </c>
     </row>
@@ -3683,7 +3692,7 @@
         <v>6.5</v>
       </c>
       <c r="H46" s="3">
-        <f>AVERAGE(C46:G46)</f>
+        <f t="shared" si="1"/>
         <v>11.3</v>
       </c>
     </row>
@@ -3710,7 +3719,7 @@
         <v>7.5</v>
       </c>
       <c r="H47" s="3">
-        <f>AVERAGE(C47:G47)</f>
+        <f t="shared" si="1"/>
         <v>11.5</v>
       </c>
     </row>
@@ -3737,7 +3746,7 @@
         <v>7.5</v>
       </c>
       <c r="H48" s="3">
-        <f>AVERAGE(C48:G48)</f>
+        <f t="shared" si="1"/>
         <v>11.6</v>
       </c>
     </row>
@@ -3764,7 +3773,7 @@
         <v>8.5</v>
       </c>
       <c r="H49" s="3">
-        <f>AVERAGE(C49:G49)</f>
+        <f t="shared" si="1"/>
         <v>11.65</v>
       </c>
     </row>
@@ -3791,7 +3800,7 @@
         <v>4.25</v>
       </c>
       <c r="H50" s="3">
-        <f>AVERAGE(C50:G50)</f>
+        <f t="shared" si="1"/>
         <v>11.7</v>
       </c>
     </row>
@@ -3818,7 +3827,7 @@
         <v>4.25</v>
       </c>
       <c r="H51" s="3">
-        <f>AVERAGE(C51:G51)</f>
+        <f t="shared" si="1"/>
         <v>11.7</v>
       </c>
     </row>
@@ -3845,7 +3854,7 @@
         <v>5.5</v>
       </c>
       <c r="H52" s="3">
-        <f>AVERAGE(C52:G52)</f>
+        <f t="shared" si="1"/>
         <v>12.05</v>
       </c>
     </row>
@@ -3872,7 +3881,7 @@
         <v>4.75</v>
       </c>
       <c r="H53" s="3">
-        <f>AVERAGE(C53:G53)</f>
+        <f t="shared" si="1"/>
         <v>12.6</v>
       </c>
     </row>
@@ -3899,7 +3908,7 @@
         <v>8.5</v>
       </c>
       <c r="H54" s="3">
-        <f>AVERAGE(C54:G54)</f>
+        <f t="shared" si="1"/>
         <v>13.4</v>
       </c>
     </row>
@@ -3926,7 +3935,7 @@
         <v>8.5</v>
       </c>
       <c r="H55" s="3">
-        <f>AVERAGE(C55:G55)</f>
+        <f t="shared" si="1"/>
         <v>13.7</v>
       </c>
     </row>
@@ -3953,7 +3962,7 @@
         <v>10.75</v>
       </c>
       <c r="H56" s="3">
-        <f>AVERAGE(C56:G56)</f>
+        <f t="shared" si="1"/>
         <v>13.9</v>
       </c>
     </row>
@@ -3980,7 +3989,7 @@
         <v>9.75</v>
       </c>
       <c r="H57" s="3">
-        <f>AVERAGE(C57:G57)</f>
+        <f t="shared" si="1"/>
         <v>13.95</v>
       </c>
     </row>
@@ -4007,7 +4016,7 @@
         <v>10</v>
       </c>
       <c r="H58" s="3">
-        <f>AVERAGE(C58:G58)</f>
+        <f t="shared" si="1"/>
         <v>14.35</v>
       </c>
     </row>
@@ -4034,7 +4043,7 @@
         <v>12</v>
       </c>
       <c r="H59" s="3">
-        <f>AVERAGE(C59:G59)</f>
+        <f t="shared" si="1"/>
         <v>14.4</v>
       </c>
     </row>
@@ -4061,7 +4070,7 @@
         <v>12</v>
       </c>
       <c r="H60" s="3">
-        <f>AVERAGE(C60:G60)</f>
+        <f t="shared" si="1"/>
         <v>14.4</v>
       </c>
     </row>
@@ -4088,7 +4097,7 @@
         <v>12.75</v>
       </c>
       <c r="H61" s="3">
-        <f>AVERAGE(C61:G61)</f>
+        <f t="shared" si="1"/>
         <v>14.65</v>
       </c>
     </row>
@@ -4115,7 +4124,7 @@
         <v>11.5</v>
       </c>
       <c r="H62" s="3">
-        <f>AVERAGE(C62:G62)</f>
+        <f t="shared" si="1"/>
         <v>15.95</v>
       </c>
     </row>
@@ -4142,7 +4151,7 @@
         <v>11.5</v>
       </c>
       <c r="H63" s="3">
-        <f>AVERAGE(C63:G63)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
@@ -4169,7 +4178,7 @@
         <v>14.25</v>
       </c>
       <c r="H64" s="3">
-        <f>AVERAGE(C64:G64)</f>
+        <f t="shared" si="1"/>
         <v>16.7</v>
       </c>
     </row>
@@ -4196,7 +4205,7 @@
         <v>20.75</v>
       </c>
       <c r="H65" s="3">
-        <f>AVERAGE(C65:G65)</f>
+        <f t="shared" si="1"/>
         <v>19.8</v>
       </c>
     </row>
@@ -4215,7 +4224,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4274,7 +4283,7 @@
         <v>18.5</v>
       </c>
       <c r="H2" s="3">
-        <f>AVERAGE(C2:G2)</f>
+        <f t="shared" ref="H2:H33" si="0">AVERAGE(C2:G2)</f>
         <v>28.05</v>
       </c>
     </row>
@@ -4301,7 +4310,7 @@
         <v>23</v>
       </c>
       <c r="H3" s="3">
-        <f>AVERAGE(C3:G3)</f>
+        <f t="shared" si="0"/>
         <v>28.95</v>
       </c>
     </row>
@@ -4328,7 +4337,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="3">
-        <f>AVERAGE(C4:G4)</f>
+        <f t="shared" si="0"/>
         <v>29.85</v>
       </c>
     </row>
@@ -4355,7 +4364,7 @@
         <v>24.75</v>
       </c>
       <c r="H5" s="3">
-        <f>AVERAGE(C5:G5)</f>
+        <f t="shared" si="0"/>
         <v>30.85</v>
       </c>
     </row>
@@ -4382,7 +4391,7 @@
         <v>18.5</v>
       </c>
       <c r="H6" s="3">
-        <f>AVERAGE(C6:G6)</f>
+        <f t="shared" si="0"/>
         <v>31.1</v>
       </c>
     </row>
@@ -4390,7 +4399,7 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C7">
@@ -4409,7 +4418,7 @@
         <v>19</v>
       </c>
       <c r="H7" s="3">
-        <f>AVERAGE(C7:G7)</f>
+        <f t="shared" si="0"/>
         <v>31.2</v>
       </c>
     </row>
@@ -4436,7 +4445,7 @@
         <v>17.25</v>
       </c>
       <c r="H8" s="3">
-        <f>AVERAGE(C8:G8)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
@@ -4463,7 +4472,7 @@
         <v>22.25</v>
       </c>
       <c r="H9" s="3">
-        <f>AVERAGE(C9:G9)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
@@ -4490,7 +4499,7 @@
         <v>23</v>
       </c>
       <c r="H10" s="3">
-        <f>AVERAGE(C10:G10)</f>
+        <f t="shared" si="0"/>
         <v>34.200000000000003</v>
       </c>
     </row>
@@ -4517,7 +4526,7 @@
         <v>28.75</v>
       </c>
       <c r="H11" s="3">
-        <f>AVERAGE(C11:G11)</f>
+        <f t="shared" si="0"/>
         <v>35.35</v>
       </c>
     </row>
@@ -4544,7 +4553,7 @@
         <v>112.25</v>
       </c>
       <c r="H12" s="3">
-        <f>AVERAGE(C12:G12)</f>
+        <f t="shared" si="0"/>
         <v>48.5</v>
       </c>
     </row>
@@ -4571,7 +4580,7 @@
         <v>122.75</v>
       </c>
       <c r="H13" s="3">
-        <f>AVERAGE(C13:G13)</f>
+        <f t="shared" si="0"/>
         <v>50.45</v>
       </c>
     </row>
@@ -4598,7 +4607,7 @@
         <v>112.25</v>
       </c>
       <c r="H14" s="3">
-        <f>AVERAGE(C14:G14)</f>
+        <f t="shared" si="0"/>
         <v>56.7</v>
       </c>
     </row>
@@ -4625,7 +4634,7 @@
         <v>142.75</v>
       </c>
       <c r="H15" s="3">
-        <f>AVERAGE(C15:G15)</f>
+        <f t="shared" si="0"/>
         <v>59.25</v>
       </c>
     </row>
@@ -4652,7 +4661,7 @@
         <v>266.75</v>
       </c>
       <c r="H16" s="3">
-        <f>AVERAGE(C16:G16)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
@@ -4679,7 +4688,7 @@
         <v>316</v>
       </c>
       <c r="H17" s="3">
-        <f>AVERAGE(C17:G17)</f>
+        <f t="shared" si="0"/>
         <v>87.45</v>
       </c>
     </row>
@@ -4706,7 +4715,7 @@
         <v>266.75</v>
       </c>
       <c r="H18" s="3">
-        <f>AVERAGE(C18:G18)</f>
+        <f t="shared" si="0"/>
         <v>87.6</v>
       </c>
     </row>
@@ -4733,7 +4742,7 @@
         <v>337.75</v>
       </c>
       <c r="H19" s="3">
-        <f>AVERAGE(C19:G19)</f>
+        <f t="shared" si="0"/>
         <v>92.1</v>
       </c>
     </row>
@@ -4760,7 +4769,7 @@
         <v>337.75</v>
       </c>
       <c r="H20" s="3">
-        <f>AVERAGE(C20:G20)</f>
+        <f t="shared" si="0"/>
         <v>92.1</v>
       </c>
     </row>
@@ -4787,7 +4796,7 @@
         <v>414.5</v>
       </c>
       <c r="H21" s="3">
-        <f>AVERAGE(C21:G21)</f>
+        <f t="shared" si="0"/>
         <v>106.55</v>
       </c>
     </row>
@@ -4814,7 +4823,7 @@
         <v>414.5</v>
       </c>
       <c r="H22" s="3">
-        <f>AVERAGE(C22:G22)</f>
+        <f t="shared" si="0"/>
         <v>107.45</v>
       </c>
     </row>
@@ -4841,7 +4850,7 @@
         <v>782.75</v>
       </c>
       <c r="H23" s="3">
-        <f>AVERAGE(C23:G23)</f>
+        <f t="shared" si="0"/>
         <v>181.1</v>
       </c>
     </row>
@@ -4868,7 +4877,7 @@
         <v>782.75</v>
       </c>
       <c r="H24" s="3">
-        <f>AVERAGE(C24:G24)</f>
+        <f t="shared" si="0"/>
         <v>187.25</v>
       </c>
     </row>
@@ -4895,7 +4904,7 @@
         <v>821.5</v>
       </c>
       <c r="H25" s="3">
-        <f>AVERAGE(C25:G25)</f>
+        <f t="shared" si="0"/>
         <v>188.55</v>
       </c>
     </row>
@@ -4922,7 +4931,7 @@
         <v>804.5</v>
       </c>
       <c r="H26" s="3">
-        <f>AVERAGE(C26:G26)</f>
+        <f t="shared" si="0"/>
         <v>197.2</v>
       </c>
     </row>
@@ -4949,7 +4958,7 @@
         <v>804.5</v>
       </c>
       <c r="H27" s="3">
-        <f>AVERAGE(C27:G27)</f>
+        <f t="shared" si="0"/>
         <v>197.7</v>
       </c>
     </row>
@@ -4976,7 +4985,7 @@
         <v>821.5</v>
       </c>
       <c r="H28" s="3">
-        <f>AVERAGE(C28:G28)</f>
+        <f t="shared" si="0"/>
         <v>200.6</v>
       </c>
     </row>
@@ -5003,7 +5012,7 @@
         <v>835.75</v>
       </c>
       <c r="H29" s="3">
-        <f>AVERAGE(C29:G29)</f>
+        <f t="shared" si="0"/>
         <v>203.95</v>
       </c>
     </row>
@@ -5030,7 +5039,7 @@
         <v>936.25</v>
       </c>
       <c r="H30" s="3">
-        <f>AVERAGE(C30:G30)</f>
+        <f t="shared" si="0"/>
         <v>227.75</v>
       </c>
     </row>
@@ -5057,7 +5066,7 @@
         <v>936.25</v>
       </c>
       <c r="H31" s="3">
-        <f>AVERAGE(C31:G31)</f>
+        <f t="shared" si="0"/>
         <v>228.35</v>
       </c>
     </row>
@@ -5084,7 +5093,7 @@
         <v>942.5</v>
       </c>
       <c r="H32" s="3">
-        <f>AVERAGE(C32:G32)</f>
+        <f t="shared" si="0"/>
         <v>229</v>
       </c>
     </row>
@@ -5111,7 +5120,7 @@
         <v>942.5</v>
       </c>
       <c r="H33" s="3">
-        <f>AVERAGE(C33:G33)</f>
+        <f t="shared" si="0"/>
         <v>229.6</v>
       </c>
     </row>
@@ -5138,7 +5147,7 @@
         <v>16</v>
       </c>
       <c r="H34" s="3">
-        <f>AVERAGE(C34:G34)</f>
+        <f t="shared" ref="H34:H65" si="1">AVERAGE(C34:G34)</f>
         <v>409.35</v>
       </c>
     </row>
@@ -5165,7 +5174,7 @@
         <v>16.5</v>
       </c>
       <c r="H35" s="3">
-        <f>AVERAGE(C35:G35)</f>
+        <f t="shared" si="1"/>
         <v>409.45</v>
       </c>
     </row>
@@ -5192,7 +5201,7 @@
         <v>27.75</v>
       </c>
       <c r="H36" s="3">
-        <f>AVERAGE(C36:G36)</f>
+        <f t="shared" si="1"/>
         <v>433.2</v>
       </c>
     </row>
@@ -5219,7 +5228,7 @@
         <v>16</v>
       </c>
       <c r="H37" s="3">
-        <f>AVERAGE(C37:G37)</f>
+        <f t="shared" si="1"/>
         <v>448.5</v>
       </c>
     </row>
@@ -5246,7 +5255,7 @@
         <v>16.5</v>
       </c>
       <c r="H38" s="3">
-        <f>AVERAGE(C38:G38)</f>
+        <f t="shared" si="1"/>
         <v>448.6</v>
       </c>
     </row>
@@ -5273,7 +5282,7 @@
         <v>16</v>
       </c>
       <c r="H39" s="3">
-        <f>AVERAGE(C39:G39)</f>
+        <f t="shared" si="1"/>
         <v>452.05</v>
       </c>
     </row>
@@ -5300,7 +5309,7 @@
         <v>16.5</v>
       </c>
       <c r="H40" s="3">
-        <f>AVERAGE(C40:G40)</f>
+        <f t="shared" si="1"/>
         <v>452.15</v>
       </c>
     </row>
@@ -5327,7 +5336,7 @@
         <v>146.5</v>
       </c>
       <c r="H41" s="3">
-        <f>AVERAGE(C41:G41)</f>
+        <f t="shared" si="1"/>
         <v>456.95</v>
       </c>
     </row>
@@ -5354,7 +5363,7 @@
         <v>16</v>
       </c>
       <c r="H42" s="3">
-        <f>AVERAGE(C42:G42)</f>
+        <f t="shared" si="1"/>
         <v>458.2</v>
       </c>
     </row>
@@ -5381,7 +5390,7 @@
         <v>16.5</v>
       </c>
       <c r="H43" s="3">
-        <f>AVERAGE(C43:G43)</f>
+        <f t="shared" si="1"/>
         <v>458.3</v>
       </c>
     </row>
@@ -5408,7 +5417,7 @@
         <v>24.75</v>
       </c>
       <c r="H44" s="3">
-        <f>AVERAGE(C44:G44)</f>
+        <f t="shared" si="1"/>
         <v>470.4</v>
       </c>
     </row>
@@ -5435,7 +5444,7 @@
         <v>25</v>
       </c>
       <c r="H45" s="3">
-        <f>AVERAGE(C45:G45)</f>
+        <f t="shared" si="1"/>
         <v>485.3</v>
       </c>
     </row>
@@ -5462,7 +5471,7 @@
         <v>17.25</v>
       </c>
       <c r="H46" s="3">
-        <f>AVERAGE(C46:G46)</f>
+        <f t="shared" si="1"/>
         <v>486.7</v>
       </c>
     </row>
@@ -5489,7 +5498,7 @@
         <v>27.5</v>
       </c>
       <c r="H47" s="3">
-        <f>AVERAGE(C47:G47)</f>
+        <f t="shared" si="1"/>
         <v>488.75</v>
       </c>
     </row>
@@ -5516,7 +5525,7 @@
         <v>122.75</v>
       </c>
       <c r="H48" s="3">
-        <f>AVERAGE(C48:G48)</f>
+        <f t="shared" si="1"/>
         <v>490</v>
       </c>
     </row>
@@ -5543,7 +5552,7 @@
         <v>142.75</v>
       </c>
       <c r="H49" s="3">
-        <f>AVERAGE(C49:G49)</f>
+        <f t="shared" si="1"/>
         <v>508.85</v>
       </c>
     </row>
@@ -5570,7 +5579,7 @@
         <v>17.25</v>
       </c>
       <c r="H50" s="3">
-        <f>AVERAGE(C50:G50)</f>
+        <f t="shared" si="1"/>
         <v>737.65</v>
       </c>
     </row>
@@ -5597,7 +5606,7 @@
         <v>21.75</v>
       </c>
       <c r="H51" s="3">
-        <f>AVERAGE(C51:G51)</f>
+        <f t="shared" si="1"/>
         <v>738.55</v>
       </c>
     </row>
@@ -5624,7 +5633,7 @@
         <v>17.25</v>
       </c>
       <c r="H52" s="3">
-        <f>AVERAGE(C52:G52)</f>
+        <f t="shared" si="1"/>
         <v>745.9</v>
       </c>
     </row>
@@ -5651,7 +5660,7 @@
         <v>21.75</v>
       </c>
       <c r="H53" s="3">
-        <f>AVERAGE(C53:G53)</f>
+        <f t="shared" si="1"/>
         <v>746.8</v>
       </c>
     </row>
@@ -5678,7 +5687,7 @@
         <v>28.75</v>
       </c>
       <c r="H54" s="3">
-        <f>AVERAGE(C54:G54)</f>
+        <f t="shared" si="1"/>
         <v>889.5</v>
       </c>
     </row>
@@ -5705,7 +5714,7 @@
         <v>146.5</v>
       </c>
       <c r="H55" s="3">
-        <f>AVERAGE(C55:G55)</f>
+        <f t="shared" si="1"/>
         <v>901.75</v>
       </c>
     </row>
@@ -5732,7 +5741,7 @@
         <v>22.25</v>
       </c>
       <c r="H56" s="3">
-        <f>AVERAGE(C56:G56)</f>
+        <f t="shared" si="1"/>
         <v>934.65</v>
       </c>
     </row>
@@ -5759,7 +5768,7 @@
         <v>27.5</v>
       </c>
       <c r="H57" s="3">
-        <f>AVERAGE(C57:G57)</f>
+        <f t="shared" si="1"/>
         <v>935.7</v>
       </c>
     </row>
@@ -5786,7 +5795,7 @@
         <v>316</v>
       </c>
       <c r="H58" s="3">
-        <f>AVERAGE(C58:G58)</f>
+        <f t="shared" si="1"/>
         <v>946.95</v>
       </c>
     </row>
@@ -5813,7 +5822,7 @@
         <v>25</v>
       </c>
       <c r="H59" s="3">
-        <f>AVERAGE(C59:G59)</f>
+        <f t="shared" si="1"/>
         <v>956.25</v>
       </c>
     </row>
@@ -5840,7 +5849,7 @@
         <v>27.75</v>
       </c>
       <c r="H60" s="3">
-        <f>AVERAGE(C60:G60)</f>
+        <f t="shared" si="1"/>
         <v>956.8</v>
       </c>
     </row>
@@ -5867,7 +5876,7 @@
         <v>835.75</v>
       </c>
       <c r="H61" s="3">
-        <f>AVERAGE(C61:G61)</f>
+        <f t="shared" si="1"/>
         <v>1039.5999999999999</v>
       </c>
     </row>
@@ -5894,7 +5903,7 @@
         <v>1619.75</v>
       </c>
       <c r="H62" s="3">
-        <f>AVERAGE(C62:G62)</f>
+        <f t="shared" si="1"/>
         <v>1574.9</v>
       </c>
     </row>
@@ -5921,7 +5930,7 @@
         <v>1619.75</v>
       </c>
       <c r="H63" s="3">
-        <f>AVERAGE(C63:G63)</f>
+        <f t="shared" si="1"/>
         <v>1574.9</v>
       </c>
     </row>
@@ -5948,7 +5957,7 @@
         <v>1699</v>
       </c>
       <c r="H64" s="3">
-        <f>AVERAGE(C64:G64)</f>
+        <f t="shared" si="1"/>
         <v>1610.25</v>
       </c>
     </row>
@@ -5975,7 +5984,7 @@
         <v>1699</v>
       </c>
       <c r="H65" s="3">
-        <f>AVERAGE(C65:G65)</f>
+        <f t="shared" si="1"/>
         <v>1610.25</v>
       </c>
     </row>
@@ -5994,7 +6003,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6053,7 +6062,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="3">
-        <f>AVERAGE(C2:G2)</f>
+        <f t="shared" ref="H2:H33" si="0">AVERAGE(C2:G2)</f>
         <v>10</v>
       </c>
     </row>
@@ -6080,7 +6089,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="3">
-        <f>AVERAGE(C3:G3)</f>
+        <f t="shared" si="0"/>
         <v>11.45</v>
       </c>
     </row>
@@ -6088,7 +6097,7 @@
       <c r="A4" s="3">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C4">
@@ -6107,7 +6116,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="3">
-        <f>AVERAGE(C4:G4)</f>
+        <f t="shared" si="0"/>
         <v>11.55</v>
       </c>
     </row>
@@ -6134,7 +6143,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="3">
-        <f>AVERAGE(C5:G5)</f>
+        <f t="shared" si="0"/>
         <v>12.15</v>
       </c>
     </row>
@@ -6161,7 +6170,7 @@
         <v>8.25</v>
       </c>
       <c r="H6" s="3">
-        <f>AVERAGE(C6:G6)</f>
+        <f t="shared" si="0"/>
         <v>12.2</v>
       </c>
     </row>
@@ -6169,7 +6178,7 @@
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -6188,7 +6197,7 @@
         <v>8.25</v>
       </c>
       <c r="H7" s="3">
-        <f>AVERAGE(C7:G7)</f>
+        <f t="shared" si="0"/>
         <v>12.7</v>
       </c>
     </row>
@@ -6215,7 +6224,7 @@
         <v>8.25</v>
       </c>
       <c r="H8" s="3">
-        <f>AVERAGE(C8:G8)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
@@ -6242,7 +6251,7 @@
         <v>8.25</v>
       </c>
       <c r="H9" s="3">
-        <f>AVERAGE(C9:G9)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
@@ -6269,7 +6278,7 @@
         <v>12</v>
       </c>
       <c r="H10" s="3">
-        <f>AVERAGE(C10:G10)</f>
+        <f t="shared" si="0"/>
         <v>13.15</v>
       </c>
     </row>
@@ -6296,7 +6305,7 @@
         <v>11.25</v>
       </c>
       <c r="H11" s="3">
-        <f>AVERAGE(C11:G11)</f>
+        <f t="shared" si="0"/>
         <v>13.45</v>
       </c>
     </row>
@@ -6323,7 +6332,7 @@
         <v>13</v>
       </c>
       <c r="H12" s="3">
-        <f>AVERAGE(C12:G12)</f>
+        <f t="shared" si="0"/>
         <v>14.35</v>
       </c>
     </row>
@@ -6350,7 +6359,7 @@
         <v>13</v>
       </c>
       <c r="H13" s="3">
-        <f>AVERAGE(C13:G13)</f>
+        <f t="shared" si="0"/>
         <v>14.9</v>
       </c>
     </row>
@@ -6377,7 +6386,7 @@
         <v>13</v>
       </c>
       <c r="H14" s="3">
-        <f>AVERAGE(C14:G14)</f>
+        <f t="shared" si="0"/>
         <v>15.7</v>
       </c>
     </row>
@@ -6404,7 +6413,7 @@
         <v>13.75</v>
       </c>
       <c r="H15" s="3">
-        <f>AVERAGE(C15:G15)</f>
+        <f t="shared" si="0"/>
         <v>15.75</v>
       </c>
     </row>
@@ -6431,7 +6440,7 @@
         <v>13.75</v>
       </c>
       <c r="H16" s="3">
-        <f>AVERAGE(C16:G16)</f>
+        <f t="shared" si="0"/>
         <v>15.85</v>
       </c>
     </row>
@@ -6458,7 +6467,7 @@
         <v>14.75</v>
       </c>
       <c r="H17" s="3">
-        <f>AVERAGE(C17:G17)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
@@ -6485,7 +6494,7 @@
         <v>13.25</v>
       </c>
       <c r="H18" s="3">
-        <f>AVERAGE(C18:G18)</f>
+        <f t="shared" si="0"/>
         <v>16.100000000000001</v>
       </c>
     </row>
@@ -6512,7 +6521,7 @@
         <v>14.75</v>
       </c>
       <c r="H19" s="3">
-        <f>AVERAGE(C19:G19)</f>
+        <f t="shared" si="0"/>
         <v>16.850000000000001</v>
       </c>
     </row>
@@ -6539,7 +6548,7 @@
         <v>14</v>
       </c>
       <c r="H20" s="3">
-        <f>AVERAGE(C20:G20)</f>
+        <f t="shared" si="0"/>
         <v>16.850000000000001</v>
       </c>
     </row>
@@ -6566,7 +6575,7 @@
         <v>14</v>
       </c>
       <c r="H21" s="3">
-        <f>AVERAGE(C21:G21)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
@@ -6593,7 +6602,7 @@
         <v>16.25</v>
       </c>
       <c r="H22" s="3">
-        <f>AVERAGE(C22:G22)</f>
+        <f t="shared" si="0"/>
         <v>17.45</v>
       </c>
     </row>
@@ -6620,7 +6629,7 @@
         <v>16.25</v>
       </c>
       <c r="H23" s="3">
-        <f>AVERAGE(C23:G23)</f>
+        <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
     </row>
@@ -6647,7 +6656,7 @@
         <v>14.75</v>
       </c>
       <c r="H24" s="3">
-        <f>AVERAGE(C24:G24)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -6674,7 +6683,7 @@
         <v>12</v>
       </c>
       <c r="H25" s="3">
-        <f>AVERAGE(C25:G25)</f>
+        <f t="shared" si="0"/>
         <v>42.6</v>
       </c>
     </row>
@@ -6701,7 +6710,7 @@
         <v>11.25</v>
       </c>
       <c r="H26" s="3">
-        <f>AVERAGE(C26:G26)</f>
+        <f t="shared" si="0"/>
         <v>44.55</v>
       </c>
     </row>
@@ -6728,7 +6737,7 @@
         <v>13</v>
       </c>
       <c r="H27" s="3">
-        <f>AVERAGE(C27:G27)</f>
+        <f t="shared" si="0"/>
         <v>44.9</v>
       </c>
     </row>
@@ -6755,7 +6764,7 @@
         <v>13.25</v>
       </c>
       <c r="H28" s="3">
-        <f>AVERAGE(C28:G28)</f>
+        <f t="shared" si="0"/>
         <v>45.7</v>
       </c>
     </row>
@@ -6782,7 +6791,7 @@
         <v>14.75</v>
       </c>
       <c r="H29" s="3">
-        <f>AVERAGE(C29:G29)</f>
+        <f t="shared" si="0"/>
         <v>46.5</v>
       </c>
     </row>
@@ -6809,7 +6818,7 @@
         <v>17.5</v>
       </c>
       <c r="H30" s="3">
-        <f>AVERAGE(C30:G30)</f>
+        <f t="shared" si="0"/>
         <v>51.2</v>
       </c>
     </row>
@@ -6836,7 +6845,7 @@
         <v>18</v>
       </c>
       <c r="H31" s="3">
-        <f>AVERAGE(C31:G31)</f>
+        <f t="shared" si="0"/>
         <v>53.3</v>
       </c>
     </row>
@@ -6863,7 +6872,7 @@
         <v>18</v>
       </c>
       <c r="H32" s="3">
-        <f>AVERAGE(C32:G32)</f>
+        <f t="shared" si="0"/>
         <v>53.55</v>
       </c>
     </row>
@@ -6890,7 +6899,7 @@
         <v>17.5</v>
       </c>
       <c r="H33" s="3">
-        <f>AVERAGE(C33:G33)</f>
+        <f t="shared" si="0"/>
         <v>56.05</v>
       </c>
     </row>
@@ -6917,7 +6926,7 @@
         <v>203.5</v>
       </c>
       <c r="H34" s="3">
-        <f>AVERAGE(C34:G34)</f>
+        <f t="shared" ref="H34:H65" si="1">AVERAGE(C34:G34)</f>
         <v>166.2</v>
       </c>
     </row>
@@ -6944,7 +6953,7 @@
         <v>369.25</v>
       </c>
       <c r="H35" s="3">
-        <f>AVERAGE(C35:G35)</f>
+        <f t="shared" si="1"/>
         <v>176.55</v>
       </c>
     </row>
@@ -6971,7 +6980,7 @@
         <v>202.75</v>
       </c>
       <c r="H36" s="3">
-        <f>AVERAGE(C36:G36)</f>
+        <f t="shared" si="1"/>
         <v>176.95</v>
       </c>
     </row>
@@ -6998,7 +7007,7 @@
         <v>202.75</v>
       </c>
       <c r="H37" s="3">
-        <f>AVERAGE(C37:G37)</f>
+        <f t="shared" si="1"/>
         <v>179.75</v>
       </c>
     </row>
@@ -7025,7 +7034,7 @@
         <v>203.5</v>
       </c>
       <c r="H38" s="3">
-        <f>AVERAGE(C38:G38)</f>
+        <f t="shared" si="1"/>
         <v>187.85</v>
       </c>
     </row>
@@ -7052,7 +7061,7 @@
         <v>216.75</v>
       </c>
       <c r="H39" s="3">
-        <f>AVERAGE(C39:G39)</f>
+        <f t="shared" si="1"/>
         <v>188.2</v>
       </c>
     </row>
@@ -7079,7 +7088,7 @@
         <v>261</v>
       </c>
       <c r="H40" s="3">
-        <f>AVERAGE(C40:G40)</f>
+        <f t="shared" si="1"/>
         <v>190.6</v>
       </c>
     </row>
@@ -7106,7 +7115,7 @@
         <v>216.75</v>
       </c>
       <c r="H41" s="3">
-        <f>AVERAGE(C41:G41)</f>
+        <f t="shared" si="1"/>
         <v>194.25</v>
       </c>
     </row>
@@ -7133,7 +7142,7 @@
         <v>315.25</v>
       </c>
       <c r="H42" s="3">
-        <f>AVERAGE(C42:G42)</f>
+        <f t="shared" si="1"/>
         <v>198.25</v>
       </c>
     </row>
@@ -7160,7 +7169,7 @@
         <v>301.25</v>
       </c>
       <c r="H43" s="3">
-        <f>AVERAGE(C43:G43)</f>
+        <f t="shared" si="1"/>
         <v>205.75</v>
       </c>
     </row>
@@ -7187,7 +7196,7 @@
         <v>228.75</v>
       </c>
       <c r="H44" s="3">
-        <f>AVERAGE(C44:G44)</f>
+        <f t="shared" si="1"/>
         <v>206.45</v>
       </c>
     </row>
@@ -7214,7 +7223,7 @@
         <v>228.75</v>
       </c>
       <c r="H45" s="3">
-        <f>AVERAGE(C45:G45)</f>
+        <f t="shared" si="1"/>
         <v>209</v>
       </c>
     </row>
@@ -7241,7 +7250,7 @@
         <v>301.25</v>
       </c>
       <c r="H46" s="3">
-        <f>AVERAGE(C46:G46)</f>
+        <f t="shared" si="1"/>
         <v>210.5</v>
       </c>
     </row>
@@ -7268,7 +7277,7 @@
         <v>354.25</v>
       </c>
       <c r="H47" s="3">
-        <f>AVERAGE(C47:G47)</f>
+        <f t="shared" si="1"/>
         <v>211.3</v>
       </c>
     </row>
@@ -7295,7 +7304,7 @@
         <v>315.25</v>
       </c>
       <c r="H48" s="3">
-        <f>AVERAGE(C48:G48)</f>
+        <f t="shared" si="1"/>
         <v>216.4</v>
       </c>
     </row>
@@ -7322,7 +7331,7 @@
         <v>251.25</v>
       </c>
       <c r="H49" s="3">
-        <f>AVERAGE(C49:G49)</f>
+        <f t="shared" si="1"/>
         <v>216.45</v>
       </c>
     </row>
@@ -7349,7 +7358,7 @@
         <v>251.25</v>
       </c>
       <c r="H50" s="3">
-        <f>AVERAGE(C50:G50)</f>
+        <f t="shared" si="1"/>
         <v>221.25</v>
       </c>
     </row>
@@ -7376,7 +7385,7 @@
         <v>260</v>
       </c>
       <c r="H51" s="3">
-        <f>AVERAGE(C51:G51)</f>
+        <f t="shared" si="1"/>
         <v>222.25</v>
       </c>
     </row>
@@ -7403,7 +7412,7 @@
         <v>369.25</v>
       </c>
       <c r="H52" s="3">
-        <f>AVERAGE(C52:G52)</f>
+        <f t="shared" si="1"/>
         <v>222.4</v>
       </c>
     </row>
@@ -7430,7 +7439,7 @@
         <v>261</v>
       </c>
       <c r="H53" s="3">
-        <f>AVERAGE(C53:G53)</f>
+        <f t="shared" si="1"/>
         <v>228.55</v>
       </c>
     </row>
@@ -7457,7 +7466,7 @@
         <v>260</v>
       </c>
       <c r="H54" s="3">
-        <f>AVERAGE(C54:G54)</f>
+        <f t="shared" si="1"/>
         <v>230.55</v>
       </c>
     </row>
@@ -7484,7 +7493,7 @@
         <v>277</v>
       </c>
       <c r="H55" s="3">
-        <f>AVERAGE(C55:G55)</f>
+        <f t="shared" si="1"/>
         <v>232.5</v>
       </c>
     </row>
@@ -7511,7 +7520,7 @@
         <v>277</v>
       </c>
       <c r="H56" s="3">
-        <f>AVERAGE(C56:G56)</f>
+        <f t="shared" si="1"/>
         <v>235.6</v>
       </c>
     </row>
@@ -7538,7 +7547,7 @@
         <v>412</v>
       </c>
       <c r="H57" s="3">
-        <f>AVERAGE(C57:G57)</f>
+        <f t="shared" si="1"/>
         <v>245.2</v>
       </c>
     </row>
@@ -7565,7 +7574,7 @@
         <v>423</v>
       </c>
       <c r="H58" s="3">
-        <f>AVERAGE(C58:G58)</f>
+        <f t="shared" si="1"/>
         <v>245.4</v>
       </c>
     </row>
@@ -7592,7 +7601,7 @@
         <v>546</v>
       </c>
       <c r="H59" s="3">
-        <f>AVERAGE(C59:G59)</f>
+        <f t="shared" si="1"/>
         <v>265.10000000000002</v>
       </c>
     </row>
@@ -7619,7 +7628,7 @@
         <v>412</v>
       </c>
       <c r="H60" s="3">
-        <f>AVERAGE(C60:G60)</f>
+        <f t="shared" si="1"/>
         <v>267.39999999999998</v>
       </c>
     </row>
@@ -7646,7 +7655,7 @@
         <v>423</v>
       </c>
       <c r="H61" s="3">
-        <f>AVERAGE(C61:G61)</f>
+        <f t="shared" si="1"/>
         <v>273.55</v>
       </c>
     </row>
@@ -7673,7 +7682,7 @@
         <v>354.25</v>
       </c>
       <c r="H62" s="3">
-        <f>AVERAGE(C62:G62)</f>
+        <f t="shared" si="1"/>
         <v>274.85000000000002</v>
       </c>
     </row>
@@ -7700,7 +7709,7 @@
         <v>476</v>
       </c>
       <c r="H63" s="3">
-        <f>AVERAGE(C63:G63)</f>
+        <f t="shared" si="1"/>
         <v>296.89999999999998</v>
       </c>
     </row>
@@ -7727,7 +7736,7 @@
         <v>476</v>
       </c>
       <c r="H64" s="3">
-        <f>AVERAGE(C64:G64)</f>
+        <f t="shared" si="1"/>
         <v>328.65</v>
       </c>
     </row>
@@ -7754,7 +7763,7 @@
         <v>546</v>
       </c>
       <c r="H65" s="3">
-        <f>AVERAGE(C65:G65)</f>
+        <f t="shared" si="1"/>
         <v>338.6</v>
       </c>
     </row>
@@ -7772,8 +7781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7F42AC-3A5E-4D27-90CC-5E948ACB468A}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7839,7 +7848,7 @@
       <c r="A3" s="3">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C3">
@@ -7893,7 +7902,7 @@
       <c r="A5" s="3">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C5">

</xml_diff>